<commit_message>
Added Usability Testing 4 & 5 notes and updates
</commit_message>
<xml_diff>
--- a/documents/User Research/User Research_Summary.xlsx
+++ b/documents/User Research/User Research_Summary.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\all\18f\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="15160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
   </bookViews>
   <sheets>
     <sheet name="Notes&amp;Themes" sheetId="1" r:id="rId1"/>
     <sheet name="Feature Importance" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>Person 1</t>
   </si>
@@ -70,6 +72,9 @@
     <t>antibiotics, pain killers</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>some, general</t>
   </si>
   <si>
@@ -187,6 +192,9 @@
     <t>Themes/data</t>
   </si>
   <si>
+    <t>Person 6</t>
+  </si>
+  <si>
     <t>Most important</t>
   </si>
   <si>
@@ -197,6 +205,54 @@
   </si>
   <si>
     <t>arWould not use the add new, just keep using the search b</t>
+  </si>
+  <si>
+    <t>12 &amp; 9</t>
+  </si>
+  <si>
+    <t>usual, Allergies, headaches</t>
+  </si>
+  <si>
+    <t>Yes, one child has a heart condition</t>
+  </si>
+  <si>
+    <t>"just figuring it out"</t>
+  </si>
+  <si>
+    <t>Which drugs hasve interactions with her child's heart medication.</t>
+  </si>
+  <si>
+    <t>History, saving notes about past experiences with medicinesm (e.g. which allergy medicine has worked best)</t>
+  </si>
+  <si>
+    <t>Like an actual cabinet, user profiles/saving medicines and searches</t>
+  </si>
+  <si>
+    <t>would like to search by active ingredient</t>
+  </si>
+  <si>
+    <t>would use it mostly to make sure medicines she gives her son and family would not hurt them or interact</t>
+  </si>
+  <si>
+    <t>would like to write notes and keep a history</t>
+  </si>
+  <si>
+    <t>3, 1.5</t>
+  </si>
+  <si>
+    <t>Wife is a NICU nurse, she handles all of the meds and healthcare</t>
+  </si>
+  <si>
+    <t>A backup or secondary check</t>
+  </si>
+  <si>
+    <t>Would like to see what medicines and at what time family members need to take medicine as a reminder</t>
+  </si>
+  <si>
+    <t>notifications/reminder</t>
+  </si>
+  <si>
+    <t>Would never use the app since wife is a healthcare professional</t>
   </si>
 </sst>
 </file>
@@ -255,16 +311,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -349,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -561,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,23 +625,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
-    <col min="3" max="6" width="37" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="6" width="37" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="8" width="37" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -594,13 +651,19 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+        <v>31</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -608,16 +671,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="G3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -625,16 +694,22 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -642,14 +717,20 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="56">
+    </row>
+    <row r="6" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -657,14 +738,20 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" ht="28">
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -672,16 +759,22 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="56">
+      <c r="G7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -689,82 +782,107 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="28">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="28">
+        <v>51</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="42">
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="56">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -772,17 +890,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -790,54 +907,54 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -855,12 +972,12 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -872,12 +989,12 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -886,15 +1003,10 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>